<commit_message>
Adicionado conexão com o banco inicial
</commit_message>
<xml_diff>
--- a/Planejamento BD.xlsx
+++ b/Planejamento BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uppertools\UTPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29DD0D04-54B0-44FD-9BD2-739B7E1E661B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5154A7DF-F916-417D-9886-D40C11655115}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0D1C983F-FDDB-452D-A1C1-29D9CA6B1606}"/>
   </bookViews>
@@ -33,26 +33,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
-  <si>
-    <t>Atividades</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t>descricao</t>
   </si>
   <si>
-    <t>codigo</t>
-  </si>
-  <si>
     <t>data_situacao</t>
   </si>
   <si>
-    <t>complemento</t>
-  </si>
-  <si>
-    <t>tipo</t>
-  </si>
-  <si>
     <t>nome</t>
   </si>
   <si>
@@ -65,15 +53,9 @@
     <t>email</t>
   </si>
   <si>
-    <t>atividade_principal</t>
-  </si>
-  <si>
     <t>atividades_secundarias</t>
   </si>
   <si>
-    <t>qsa</t>
-  </si>
-  <si>
     <t>Pessoas</t>
   </si>
   <si>
@@ -98,9 +80,6 @@
     <t>municipio</t>
   </si>
   <si>
-    <t>porte</t>
-  </si>
-  <si>
     <t>abertura</t>
   </si>
   <si>
@@ -110,22 +89,121 @@
     <t>fantasia</t>
   </si>
   <si>
-    <t>cnpj</t>
-  </si>
-  <si>
     <t>ultima_atualizacao</t>
   </si>
   <si>
-    <t>efr</t>
-  </si>
-  <si>
     <t>capital_social</t>
   </si>
   <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Tipo</t>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>CNPJ (pk)</t>
+  </si>
+  <si>
+    <t>Endereco</t>
+  </si>
+  <si>
+    <t>Situacao</t>
+  </si>
+  <si>
+    <t>TipoEmpresa</t>
+  </si>
+  <si>
+    <t>IdTipo (fk)</t>
+  </si>
+  <si>
+    <t>Complemento</t>
+  </si>
+  <si>
+    <t>varchar(14)</t>
+  </si>
+  <si>
+    <t>varchar(255)</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>varchar(2)</t>
+  </si>
+  <si>
+    <t>IdAtividade(pk)(fk)</t>
+  </si>
+  <si>
+    <t>IdEmpresa(pk)(fk)</t>
+  </si>
+  <si>
+    <t>Atividade</t>
+  </si>
+  <si>
+    <t>Descricao</t>
+  </si>
+  <si>
+    <t>administracao</t>
+  </si>
+  <si>
+    <t>IdPessoa (pk)</t>
+  </si>
+  <si>
+    <t>IdEmpresa (pk)(fk)</t>
+  </si>
+  <si>
+    <t>IdPessoa (pk)(fk)</t>
+  </si>
+  <si>
+    <t>IdSituacao (pk)</t>
+  </si>
+  <si>
+    <t>IdSituacao(fk)</t>
+  </si>
+  <si>
+    <t>IdEndereco (pk)</t>
+  </si>
+  <si>
+    <t>IdEndereco (fk)</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>varchar(40)</t>
+  </si>
+  <si>
+    <t>codigo (pk)</t>
+  </si>
+  <si>
+    <t>codigoAt (fk)</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>varchar(10)</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>decimal(12,2)</t>
+  </si>
+  <si>
+    <t>varchar(30)</t>
+  </si>
+  <si>
+    <t>varchar(9)</t>
+  </si>
+  <si>
+    <t>varchar(80)</t>
+  </si>
+  <si>
+    <t>IdTipo (pk)</t>
+  </si>
+  <si>
+    <t>CNPJ (fk)</t>
   </si>
 </sst>
 </file>
@@ -477,164 +555,296 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47900FBF-4D43-4D56-A16D-99A1317CA594}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
       <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>28</v>
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>